<commit_message>
Added support for modifying meta tags (persistent save in file), reworked meta tag handling classes.
</commit_message>
<xml_diff>
--- a/_Docs, stuff/TODO.xlsx
+++ b/_Docs, stuff/TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Feature group</t>
   </si>
@@ -30,33 +30,15 @@
     <t>Aim week</t>
   </si>
   <si>
-    <t>Mockup UI</t>
-  </si>
-  <si>
-    <t>Implement UI</t>
-  </si>
-  <si>
-    <t>Setup MusicBrainz server</t>
-  </si>
-  <si>
     <t>Choose track fingerprint library</t>
   </si>
   <si>
-    <t>Choose ID3 tagger library</t>
-  </si>
-  <si>
-    <t>UI / UX</t>
-  </si>
-  <si>
     <t>Libraries / plugins</t>
   </si>
   <si>
     <t>Foobar2000 playlist handling</t>
   </si>
   <si>
-    <t>MusicBrainz ID3 fill by fingerprint</t>
-  </si>
-  <si>
     <t>MusicBrainz login and sync</t>
   </si>
   <si>
@@ -66,9 +48,6 @@
     <t>Offline ID3 tag sync</t>
   </si>
   <si>
-    <t>UI for track browsing</t>
-  </si>
-  <si>
     <t>UI for foobar2000 integration</t>
   </si>
   <si>
@@ -99,12 +78,6 @@
     <t>Spotify</t>
   </si>
   <si>
-    <t>Git</t>
-  </si>
-  <si>
-    <t>Git folder and workflow</t>
-  </si>
-  <si>
     <t>Algorithms</t>
   </si>
   <si>
@@ -112,6 +85,12 @@
   </si>
   <si>
     <t>Multi-user support for create shared playlist based on likes</t>
+  </si>
+  <si>
+    <t>UX / UI</t>
+  </si>
+  <si>
+    <t>MusicBrainz ID3 fill via search</t>
   </si>
 </sst>
 </file>
@@ -147,7 +126,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,8 +139,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -170,13 +155,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thick">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thick">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -191,7 +206,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thick">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -206,7 +221,7 @@
       <right style="thick">
         <color auto="1"/>
       </right>
-      <top style="thick">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -224,7 +239,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -239,7 +254,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -254,7 +269,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -269,9 +284,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -284,9 +297,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -299,87 +310,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -516,127 +447,109 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -919,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -934,206 +847,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="25"/>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4">
         <v>8</v>
       </c>
-      <c r="B2" s="28" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="26"/>
+      <c r="B5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C5" s="33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="25"/>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="23">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="30" t="s">
+    <row r="11" spans="1:3" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="30" t="s">
+      <c r="B12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="30" t="s">
+      <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="36"/>
-      <c r="B10" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="19">
+      <c r="C13" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
-      <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="40" t="s">
+    <row r="14" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="29"/>
+      <c r="B14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="15">
         <v>10</v>
       </c>
-      <c r="C16" s="41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
-      <c r="B20" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1143,42 +1030,12 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Milestone reached. Improved UI, MBAPI, AcoustID and tagging.
</commit_message>
<xml_diff>
--- a/_Docs, stuff/TODO.xlsx
+++ b/_Docs, stuff/TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Feature group</t>
   </si>
@@ -30,24 +30,12 @@
     <t>Libraries / plugins</t>
   </si>
   <si>
-    <t>Foobar2000 playlist handling</t>
-  </si>
-  <si>
-    <t>Offline ID3 tag sync</t>
-  </si>
-  <si>
     <t>UI for foobar2000 integration</t>
   </si>
   <si>
-    <t>MusicBrainz</t>
-  </si>
-  <si>
     <t>Generate statistics</t>
   </si>
   <si>
-    <t>Foobar2000</t>
-  </si>
-  <si>
     <t>UI for statistics</t>
   </si>
   <si>
@@ -63,16 +51,85 @@
     <t>Algorithms</t>
   </si>
   <si>
-    <t>Improve offline parsing based on folder or file names (albums)</t>
-  </si>
-  <si>
     <t>UX / UI</t>
   </si>
   <si>
-    <t>MusicBrainz ID3 fill via search</t>
-  </si>
-  <si>
-    <t>AcoustID fingerprinting</t>
+    <t>Comment / Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Improved drive search</t>
+  </si>
+  <si>
+    <t>Limited to external now to avoid messing with system files.</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Added fingerprinting feature (AcoustID)</t>
+  </si>
+  <si>
+    <t>Needs minor tweaks @ async implementation.</t>
+  </si>
+  <si>
+    <t>Reworked tagging mechanism internally</t>
+  </si>
+  <si>
+    <t>Faster and more structured.</t>
+  </si>
+  <si>
+    <t>Added ability to manually modify EACH tag (details too)</t>
+  </si>
+  <si>
+    <t>Internet connection status now updates every 5 sec</t>
+  </si>
+  <si>
+    <t>Need to add connection check @ webAPI calls…</t>
+  </si>
+  <si>
+    <t>Improved Tracklist UI</t>
+  </si>
+  <si>
+    <t>Further iterations required.</t>
+  </si>
+  <si>
+    <t>Added own MusicBrainz API wrapper</t>
+  </si>
+  <si>
+    <t>Debug various misterious exceptions…</t>
+  </si>
+  <si>
+    <t>Buggy</t>
+  </si>
+  <si>
+    <t>Implemented all kinds of MB query algorithms and grouping by albums</t>
+  </si>
+  <si>
+    <t>Needs to be tested after MBAPI wrapper fix (above).</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Offline ID3 tag sync and persistence periodically</t>
+  </si>
+  <si>
+    <t>UI for app settings</t>
+  </si>
+  <si>
+    <t>Improve offline parsing based on folder names (albums)</t>
+  </si>
+  <si>
+    <t>Improve mixing feature @ Playzone tab</t>
+  </si>
+  <si>
+    <t>Data structure &amp; code</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -108,15 +165,39 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -170,18 +251,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -189,47 +268,6 @@
         <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
         <color auto="1"/>
       </right>
       <top style="thick">
@@ -252,25 +290,143 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thick">
         <color auto="1"/>
       </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thick">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -283,7 +439,7 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thick">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -292,41 +448,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -334,13 +472,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -623,129 +800,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="21" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
+      <c r="B6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="21" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="B14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
-      <c r="B5" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="21" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-    </row>
+      <c r="C17" s="10"/>
+      <c r="D17" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="21" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
+  <mergeCells count="3">
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added icons to UI tabs, improved Playlist behaviour and added the future base of statistics handling.
</commit_message>
<xml_diff>
--- a/_Docs, stuff/TODO.xlsx
+++ b/_Docs, stuff/TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Feature group</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Nope</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +199,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -448,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -460,12 +469,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -478,9 +481,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -505,19 +505,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -802,9 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
@@ -819,27 +829,27 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>15</v>
       </c>
     </row>
@@ -847,13 +857,13 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -861,49 +871,49 @@
       <c r="A4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -911,13 +921,13 @@
       <c r="A8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -925,45 +935,45 @@
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="23" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="24" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="25" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="24" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="25" t="s">
         <v>36</v>
       </c>
     </row>
@@ -971,33 +981,33 @@
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="24" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="25" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="24" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="25" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="24" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="25" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1005,23 +1015,23 @@
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="24" t="s">
-        <v>36</v>
+      <c r="C16" s="7"/>
+      <c r="D16" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="25" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>